<commit_message>
User acceptance Testing completed
</commit_message>
<xml_diff>
--- a/Development/UAT.xlsx
+++ b/Development/UAT.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="124">
   <si>
     <t xml:space="preserve">User Acceptance Test Plan</t>
   </si>
@@ -188,58 +188,205 @@
     <t xml:space="preserve">admin can create a new property</t>
   </si>
   <si>
+    <t xml:space="preserve">login as admin -&gt; click on “Add accomodation type” -&gt; create and publish new property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new property is listed on the property page</t>
+  </si>
+  <si>
     <t xml:space="preserve">admin can edit any existing property</t>
   </si>
   <si>
+    <t xml:space="preserve">login as admin -&gt; switch to Accomodations tab -&gt; click “edit” on existing property -&gt; make changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">changes are being displayed on property page</t>
+  </si>
+  <si>
     <t xml:space="preserve">admin can add Categories, Tags, Amenities, Attributes, Seasons, Rates and Services</t>
   </si>
   <si>
+    <t xml:space="preserve">login as admin -&gt; switch to Accomodations tab -&gt; create new Categories, Tags, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Categories are created and can be used when generating a new property</t>
+  </si>
+  <si>
     <t xml:space="preserve">admin can delete any existing properties</t>
   </si>
   <si>
+    <t xml:space="preserve">login admin -&gt; click on Accomodation types -&gt; click on delete button of any property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">property is deleted and does not show in the property page</t>
+  </si>
+  <si>
     <t xml:space="preserve">Property Owner account can create a new property</t>
   </si>
   <si>
+    <t xml:space="preserve">login with property owner account -&gt; click on “Add accomodation type” -&gt; create and publish new property</t>
+  </si>
+  <si>
     <t xml:space="preserve">Property Owner account can edit their personal properties</t>
   </si>
   <si>
+    <t xml:space="preserve">login with property owner account -&gt; switch to Accomodations tab -&gt; click “edit” on existing personal property -&gt; make changes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Property Owner account can add Categories, Tags, Amenities, Attributes, Seasons, Rates and Services</t>
   </si>
   <si>
+    <t xml:space="preserve">login with property owner account -&gt; switch to Accomodations tab -&gt; create new Categories, Tags, etc.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Property Owner account can delete personal properties</t>
   </si>
   <si>
+    <t xml:space="preserve">login admin -&gt; click on Accomodation types -&gt; click on delete button of personal proproty</t>
+  </si>
+  <si>
     <t xml:space="preserve">BOOKING MANAGEMENT</t>
   </si>
   <si>
     <t xml:space="preserve">users that are not logged in cannot make bookings</t>
   </si>
   <si>
+    <t xml:space="preserve">select property and complete booking process without being logged in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User can view property, but cannot finish booking process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user gets redirected to login page</t>
+  </si>
+  <si>
     <t xml:space="preserve">logged in users can make complete bookings</t>
   </si>
   <si>
+    <t xml:space="preserve">select property -&gt; click on book -&gt; enter credentials -&gt; select payment type -&gt; finish booking process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User successfully finishes booking process and receives booking confirmation – booking is registered in the Booking tab of the wordpress dashboard</t>
+  </si>
+  <si>
     <t xml:space="preserve">Property Owner account can view bookings for personal properties</t>
   </si>
   <si>
+    <t xml:space="preserve">login with property owner account -&gt; switch to Booking tab -&gt; view bookings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bookings are being displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Property owners can view all bookings</t>
+  </si>
+  <si>
     <t xml:space="preserve">Property Owner account can edit bookings for personal properties </t>
   </si>
   <si>
+    <t xml:space="preserve">login with property owner account -&gt; switch to Booking tab -&gt; click on edit button under bookings for personal properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">property owner can edit bookings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">with the current version, Property Owners cannot edit bookings of other people</t>
+  </si>
+  <si>
+    <t xml:space="preserve">when enabling property owners to edit bookigns, they can do so for all bookings, even for different properties. This needs to be fixed in future updates.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Property Owner account can cancel bookings for personal properties</t>
   </si>
   <si>
+    <t xml:space="preserve">login with property owner account -&gt; switch to Booking tab -&gt; select booking -&gt; change action to “move to trash”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bookings is deleted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">with the current version, Property Owners cannot delete bookings of other people</t>
+  </si>
+  <si>
+    <t xml:space="preserve">when enabling property owners to delete bookigns, they can do so for all bookings, even for different properties. This needs to be fixed in future updates.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Property Owner account can manually create new bookings for personal properties </t>
   </si>
   <si>
-    <t xml:space="preserve">admin can view bookings for all properties</t>
+    <t xml:space="preserve">login with property owner account -&gt; switch to Booking tab -&gt; click on “add new booking” button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new bookings is added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">button cannot be pressed (Requires Pro version of hotel booking plugin)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin can view all bookings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">login as admin -&gt; switch to bookings tab -&gt; view bookings</t>
   </si>
   <si>
     <t xml:space="preserve">admin can edit bookings for all properties </t>
   </si>
   <si>
+    <t xml:space="preserve">login as admin -&gt; switch to bookings tab -&gt; click on edit button on any booking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin can edit any booking</t>
+  </si>
+  <si>
     <t xml:space="preserve">admin can cancel bookings for all properties</t>
   </si>
   <si>
+    <t xml:space="preserve">login as admin -&gt; switch to bookings tab -&gt; select bookings -&gt; perform action “move to trash”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bookingis deleted</t>
+  </si>
+  <si>
     <t xml:space="preserve">admin can manually create new bookings for all properties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">login as admin -&gt; switch to Booking tab -&gt; click on “add new booking” button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">users receive booking confirmation after booking a property</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logged in user makes a booking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a confirmation mail is sent to user that made the booking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAYMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">users receive email payment instructions for direct bank transfer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logged in user makes a booking and selects “direct bank transfer” as payment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email with instruction for the bank transfer is sent to the user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">final paying instructions need to be finished by the client</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Users can pay via Paypal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user can pay with paypal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">error when redirecting to paypal site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paypal account needs to be setup properly for it to work</t>
   </si>
   <si>
     <t xml:space="preserve">Environment Test Plan</t>
@@ -266,7 +413,7 @@
     <numFmt numFmtId="165" formatCode="d\-mmm\-yy"/>
     <numFmt numFmtId="166" formatCode="d\-mmm"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -388,6 +535,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="18"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -562,13 +721,6 @@
       <left/>
       <right style="thin"/>
       <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
-      <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
@@ -577,6 +729,13 @@
       <right style="medium"/>
       <top/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -608,7 +767,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -781,28 +940,36 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="18" fillId="3" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="2" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="2" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="3" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="3" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -891,22 +1058,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:W36"/>
+  <dimension ref="A1:W40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I40" activeCellId="0" sqref="I40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="32.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="2" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="22.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="32.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="8.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="14.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="11.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="25.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="2" width="9.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="2" width="9.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1054,7 +1222,7 @@
       <c r="I8" s="22"/>
       <c r="J8" s="22"/>
     </row>
-    <row r="9" s="19" customFormat="true" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" s="19" customFormat="true" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="23" t="n">
         <v>1</v>
       </c>
@@ -1080,7 +1248,7 @@
       <c r="I9" s="28"/>
       <c r="J9" s="28"/>
     </row>
-    <row r="10" s="19" customFormat="true" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" s="19" customFormat="true" ht="87.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="23" t="n">
         <v>2</v>
       </c>
@@ -1281,11 +1449,17 @@
       <c r="B18" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="34"/>
+      <c r="C18" s="34" t="s">
+        <v>52</v>
+      </c>
       <c r="D18" s="34"/>
       <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
+      <c r="F18" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="24" t="s">
+        <v>22</v>
+      </c>
       <c r="H18" s="27" t="s">
         <v>23</v>
       </c>
@@ -1297,15 +1471,21 @@
         <v>10</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="42"/>
+        <v>54</v>
+      </c>
+      <c r="C19" s="42" t="s">
+        <v>55</v>
+      </c>
       <c r="D19" s="42"/>
       <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="31" t="s">
-        <v>36</v>
+      <c r="F19" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="27" t="s">
+        <v>23</v>
       </c>
       <c r="I19" s="28"/>
       <c r="J19" s="28"/>
@@ -1315,14 +1495,22 @@
         <v>11</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="42"/>
+        <v>57</v>
+      </c>
+      <c r="C20" s="42" t="s">
+        <v>58</v>
+      </c>
       <c r="D20" s="42"/>
       <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="31"/>
+      <c r="F20" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="27" t="s">
+        <v>23</v>
+      </c>
       <c r="I20" s="28"/>
       <c r="J20" s="28"/>
     </row>
@@ -1331,46 +1519,70 @@
         <v>12</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="42"/>
+        <v>60</v>
+      </c>
+      <c r="C21" s="42" t="s">
+        <v>61</v>
+      </c>
       <c r="D21" s="42"/>
       <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="31"/>
+      <c r="F21" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="27" t="s">
+        <v>23</v>
+      </c>
       <c r="I21" s="29"/>
       <c r="J21" s="30"/>
     </row>
-    <row r="22" s="19" customFormat="true" ht="35.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" s="19" customFormat="true" ht="49.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="23" t="n">
         <v>13</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
+        <v>63</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="34"/>
       <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="31"/>
+      <c r="F22" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="27" t="s">
+        <v>23</v>
+      </c>
       <c r="I22" s="28"/>
       <c r="J22" s="28"/>
     </row>
-    <row r="23" s="19" customFormat="true" ht="35.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" s="19" customFormat="true" ht="54.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="23" t="n">
         <v>14</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" s="42"/>
+        <v>65</v>
+      </c>
+      <c r="C23" s="42" t="s">
+        <v>66</v>
+      </c>
       <c r="D23" s="42"/>
       <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="31"/>
+      <c r="F23" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="43" t="s">
+        <v>23</v>
+      </c>
       <c r="I23" s="28"/>
       <c r="J23" s="28"/>
     </row>
@@ -1379,14 +1591,22 @@
         <v>15</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24" s="42"/>
+        <v>67</v>
+      </c>
+      <c r="C24" s="42" t="s">
+        <v>68</v>
+      </c>
       <c r="D24" s="42"/>
       <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="31"/>
+      <c r="F24" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="G24" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="43" t="s">
+        <v>23</v>
+      </c>
       <c r="I24" s="28"/>
       <c r="J24" s="28"/>
     </row>
@@ -1395,20 +1615,28 @@
         <v>16</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" s="42"/>
+        <v>69</v>
+      </c>
+      <c r="C25" s="42" t="s">
+        <v>70</v>
+      </c>
       <c r="D25" s="42"/>
       <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="31"/>
+      <c r="F25" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G25" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="43" t="s">
+        <v>23</v>
+      </c>
       <c r="I25" s="28"/>
       <c r="J25" s="28"/>
     </row>
     <row r="26" s="19" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="40" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="22"/>
@@ -1425,30 +1653,48 @@
         <v>17</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="34"/>
+        <v>72</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>73</v>
+      </c>
       <c r="D27" s="34"/>
       <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="28"/>
+      <c r="F27" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="G27" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="I27" s="28" t="s">
+        <v>75</v>
+      </c>
       <c r="J27" s="28"/>
     </row>
-    <row r="28" s="19" customFormat="true" ht="35.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" s="19" customFormat="true" ht="68.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="23" t="n">
         <v>18</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="43"/>
+        <v>76</v>
+      </c>
+      <c r="C28" s="44" t="s">
+        <v>77</v>
+      </c>
       <c r="D28" s="44"/>
       <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="31"/>
+      <c r="F28" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="G28" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H28" s="43" t="s">
+        <v>23</v>
+      </c>
       <c r="I28" s="29"/>
       <c r="J28" s="30"/>
     </row>
@@ -1457,131 +1703,291 @@
         <v>19</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="42"/>
+        <v>79</v>
+      </c>
+      <c r="C29" s="42" t="s">
+        <v>80</v>
+      </c>
       <c r="D29" s="42"/>
       <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="30"/>
-    </row>
-    <row r="30" s="19" customFormat="true" ht="43.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F29" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="G29" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="I29" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="J29" s="32"/>
+    </row>
+    <row r="30" s="19" customFormat="true" ht="73.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="23" t="n">
         <v>20</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="42"/>
+        <v>83</v>
+      </c>
+      <c r="C30" s="42" t="s">
+        <v>84</v>
+      </c>
       <c r="D30" s="42"/>
       <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="30"/>
-    </row>
-    <row r="31" s="19" customFormat="true" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F30" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="G30" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="H30" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="I30" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="J30" s="32"/>
+    </row>
+    <row r="31" s="19" customFormat="true" ht="72.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="23" t="n">
         <v>21</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
+        <v>88</v>
+      </c>
+      <c r="C31" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" s="45"/>
       <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="28"/>
+      <c r="F31" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="G31" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="H31" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="I31" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="J31" s="32"/>
     </row>
     <row r="32" s="19" customFormat="true" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="23" t="n">
         <v>22</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="C32" s="42"/>
-      <c r="D32" s="44"/>
+        <v>93</v>
+      </c>
+      <c r="C32" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" s="45"/>
       <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="31"/>
+      <c r="F32" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="G32" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="H32" s="31" t="s">
+        <v>36</v>
+      </c>
       <c r="I32" s="28"/>
-      <c r="J32" s="30"/>
+      <c r="J32" s="28"/>
     </row>
     <row r="33" s="19" customFormat="true" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="23" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="C33" s="42"/>
+        <v>97</v>
+      </c>
+      <c r="C33" s="42" t="s">
+        <v>98</v>
+      </c>
       <c r="D33" s="42"/>
       <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="31"/>
+      <c r="F33" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="G33" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" s="43" t="s">
+        <v>23</v>
+      </c>
       <c r="I33" s="29"/>
       <c r="J33" s="30"/>
     </row>
     <row r="34" s="19" customFormat="true" ht="43.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="23" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B34" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="C34" s="42"/>
+        <v>99</v>
+      </c>
+      <c r="C34" s="42" t="s">
+        <v>100</v>
+      </c>
       <c r="D34" s="42"/>
       <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="31"/>
+      <c r="F34" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="G34" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H34" s="43" t="s">
+        <v>23</v>
+      </c>
       <c r="I34" s="29"/>
       <c r="J34" s="30"/>
     </row>
     <row r="35" s="19" customFormat="true" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="23" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="C35" s="42"/>
+        <v>102</v>
+      </c>
+      <c r="C35" s="42" t="s">
+        <v>103</v>
+      </c>
       <c r="D35" s="42"/>
       <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="31"/>
+      <c r="F35" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="G35" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" s="43" t="s">
+        <v>23</v>
+      </c>
       <c r="I35" s="28"/>
       <c r="J35" s="28"/>
     </row>
     <row r="36" s="19" customFormat="true" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="23" t="n">
+        <v>26</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" s="45"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="G36" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="H36" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="I36" s="28"/>
+      <c r="J36" s="28"/>
+    </row>
+    <row r="37" s="19" customFormat="true" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="23" t="n">
+        <v>27</v>
+      </c>
+      <c r="B37" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="34"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="G37" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="C36" s="42"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="28"/>
-      <c r="J36" s="30"/>
+      <c r="H37" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="I37" s="28"/>
+      <c r="J37" s="28"/>
+    </row>
+    <row r="38" s="19" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="B38" s="41"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+    </row>
+    <row r="39" s="19" customFormat="true" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="23" t="n">
+        <v>28</v>
+      </c>
+      <c r="B39" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="D39" s="34"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="G39" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H39" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="I39" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="J39" s="28"/>
+    </row>
+    <row r="40" s="19" customFormat="true" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="23" t="n">
+        <v>29</v>
+      </c>
+      <c r="B40" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C40" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="D40" s="34"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="G40" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="H40" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="I40" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="J40" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="55">
+  <mergeCells count="69">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:J1"/>
     <mergeCell ref="A2:B2"/>
@@ -1629,14 +2035,28 @@
     <mergeCell ref="C26:J26"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="I27:J27"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C29:D29"/>
+    <mergeCell ref="I29:J29"/>
     <mergeCell ref="C30:D30"/>
+    <mergeCell ref="I30:J30"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="I31:J31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="I32:J32"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="I35:J35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="C38:J38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="I40:J40"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.236111111111111" right="0.236111111111111" top="0.236111111111111" bottom="0.511805555555556" header="0.511811023622047" footer="0.236111111111111"/>
@@ -1659,24 +2079,24 @@
       <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.12109375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.12890625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="32.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="32.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="24.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="7.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="7.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="11.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="25.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="2" width="9.11"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="2" width="9.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="5" t="s">
-        <v>70</v>
+        <v>119</v>
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
@@ -1729,8 +2149,8 @@
         <v>7</v>
       </c>
       <c r="B5" s="6"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
@@ -1788,7 +2208,7 @@
     </row>
     <row r="8" s="19" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="20" t="s">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
@@ -1797,7 +2217,7 @@
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
-      <c r="I8" s="46"/>
+      <c r="I8" s="47"/>
     </row>
     <row r="9" s="19" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="23" t="n">
@@ -1808,9 +2228,9 @@
       <c r="D9" s="24"/>
       <c r="E9" s="24"/>
       <c r="F9" s="24"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
     </row>
     <row r="10" s="19" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="23" t="n">
@@ -1821,7 +2241,7 @@
       <c r="D10" s="34"/>
       <c r="E10" s="24"/>
       <c r="F10" s="24"/>
-      <c r="G10" s="47"/>
+      <c r="G10" s="48"/>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
     </row>
@@ -1834,7 +2254,7 @@
       <c r="D11" s="42"/>
       <c r="E11" s="24"/>
       <c r="F11" s="24"/>
-      <c r="G11" s="47"/>
+      <c r="G11" s="48"/>
       <c r="H11" s="29"/>
       <c r="I11" s="30"/>
     </row>
@@ -1847,7 +2267,7 @@
       <c r="D12" s="42"/>
       <c r="E12" s="24"/>
       <c r="F12" s="24"/>
-      <c r="G12" s="47"/>
+      <c r="G12" s="48"/>
       <c r="H12" s="29"/>
       <c r="I12" s="30"/>
     </row>
@@ -1860,13 +2280,13 @@
       <c r="D13" s="42"/>
       <c r="E13" s="24"/>
       <c r="F13" s="24"/>
-      <c r="G13" s="47"/>
+      <c r="G13" s="48"/>
       <c r="H13" s="28"/>
       <c r="I13" s="28"/>
     </row>
     <row r="14" s="19" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="20" t="s">
-        <v>72</v>
+        <v>121</v>
       </c>
       <c r="B14" s="20"/>
       <c r="C14" s="20"/>
@@ -1886,7 +2306,7 @@
       <c r="D15" s="42"/>
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
-      <c r="G15" s="47"/>
+      <c r="G15" s="48"/>
       <c r="H15" s="28"/>
       <c r="I15" s="28"/>
     </row>
@@ -1899,7 +2319,7 @@
       <c r="D16" s="42"/>
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
-      <c r="G16" s="47"/>
+      <c r="G16" s="48"/>
       <c r="H16" s="29"/>
       <c r="I16" s="30"/>
     </row>
@@ -1912,7 +2332,7 @@
       <c r="D17" s="42"/>
       <c r="E17" s="24"/>
       <c r="F17" s="24"/>
-      <c r="G17" s="47"/>
+      <c r="G17" s="48"/>
       <c r="H17" s="28"/>
       <c r="I17" s="28"/>
     </row>
@@ -1925,7 +2345,7 @@
       <c r="D18" s="42"/>
       <c r="E18" s="24"/>
       <c r="F18" s="24"/>
-      <c r="G18" s="47"/>
+      <c r="G18" s="48"/>
       <c r="H18" s="29"/>
       <c r="I18" s="30"/>
     </row>
@@ -1938,13 +2358,13 @@
       <c r="D19" s="42"/>
       <c r="E19" s="24"/>
       <c r="F19" s="24"/>
-      <c r="G19" s="47"/>
+      <c r="G19" s="48"/>
       <c r="H19" s="28"/>
       <c r="I19" s="28"/>
     </row>
     <row r="20" s="19" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="20" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
       <c r="B20" s="20"/>
       <c r="C20" s="20"/>
@@ -1964,7 +2384,7 @@
       <c r="D21" s="42"/>
       <c r="E21" s="24"/>
       <c r="F21" s="24"/>
-      <c r="G21" s="47"/>
+      <c r="G21" s="48"/>
       <c r="H21" s="28"/>
       <c r="I21" s="28"/>
     </row>
@@ -1973,11 +2393,11 @@
         <v>2</v>
       </c>
       <c r="B22" s="24"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="44"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="50"/>
       <c r="E22" s="24"/>
       <c r="F22" s="24"/>
-      <c r="G22" s="47"/>
+      <c r="G22" s="48"/>
       <c r="H22" s="29"/>
       <c r="I22" s="30"/>
     </row>
@@ -1990,7 +2410,7 @@
       <c r="D23" s="42"/>
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
-      <c r="G23" s="47"/>
+      <c r="G23" s="48"/>
       <c r="H23" s="29"/>
       <c r="I23" s="30"/>
     </row>
@@ -2003,7 +2423,7 @@
       <c r="D24" s="42"/>
       <c r="E24" s="24"/>
       <c r="F24" s="24"/>
-      <c r="G24" s="47"/>
+      <c r="G24" s="48"/>
       <c r="H24" s="29"/>
       <c r="I24" s="30"/>
     </row>
@@ -2016,33 +2436,33 @@
       <c r="D25" s="42"/>
       <c r="E25" s="24"/>
       <c r="F25" s="24"/>
-      <c r="G25" s="47"/>
+      <c r="G25" s="48"/>
       <c r="H25" s="28"/>
       <c r="I25" s="28"/>
     </row>
     <row r="26" s="19" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="B26" s="49"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="49"/>
-      <c r="H26" s="49"/>
-      <c r="I26" s="49"/>
+      <c r="A26" s="51" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" s="51"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="51"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="51"/>
+      <c r="I26" s="51"/>
     </row>
     <row r="27" s="19" customFormat="true" ht="65.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="33"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="50"/>
-      <c r="I27" s="50"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="52"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="52"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="39">

</xml_diff>